<commit_message>
feat: add fr, de i18n; ocr tool
</commit_message>
<xml_diff>
--- a/tools/data-processing/data.xlsx
+++ b/tools/data-processing/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\might-and-magic\arcomage-hd\tools\data-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8024785-DD75-42BA-93C6-2B48A206FE7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E0712D-D634-463A-8BF5-571EA1548225}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1130,9 +1130,6 @@
     <t>无影神偷</t>
   </si>
   <si>
-    <t>对手宝石-10，砖头-5，你得到其中一半</t>
-  </si>
-  <si>
     <t>岩石巨人</t>
   </si>
   <si>
@@ -1263,6 +1260,9 @@
   </si>
   <si>
     <t>对手城堡-12</t>
+  </si>
+  <si>
+    <t>对手宝石-10，砖头-5，你得到其中一半（向上取整）</t>
   </si>
 </sst>
 </file>
@@ -5225,8 +5225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85D8E1A-6405-4E81-99A0-42E9F3DFBBDB}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5333,7 +5333,7 @@
         <v>216</v>
       </c>
       <c r="F7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -5627,7 +5627,7 @@
         <v>291</v>
       </c>
       <c r="F28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -5666,10 +5666,10 @@
         <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -5680,10 +5680,10 @@
         <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -5694,10 +5694,10 @@
         <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -5708,10 +5708,10 @@
         <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F34" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -5722,10 +5722,10 @@
         <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -5935,7 +5935,7 @@
         <v>308</v>
       </c>
       <c r="F50" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -5946,7 +5946,7 @@
         <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F51" t="s">
         <v>309</v>
@@ -6103,7 +6103,7 @@
         <v>330</v>
       </c>
       <c r="F62" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -6142,10 +6142,10 @@
         <v>29</v>
       </c>
       <c r="E65" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F65" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -6156,10 +6156,10 @@
         <v>30</v>
       </c>
       <c r="E66" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F66" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -6170,10 +6170,10 @@
         <v>31</v>
       </c>
       <c r="E67" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F67" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -6184,10 +6184,10 @@
         <v>32</v>
       </c>
       <c r="E68" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F68" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -6198,10 +6198,10 @@
         <v>33</v>
       </c>
       <c r="E69" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F69" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -6299,7 +6299,7 @@
         <v>248</v>
       </c>
       <c r="F76" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -6411,7 +6411,7 @@
         <v>346</v>
       </c>
       <c r="F84" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -6509,7 +6509,7 @@
         <v>359</v>
       </c>
       <c r="F91" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -6565,7 +6565,7 @@
         <v>366</v>
       </c>
       <c r="F95" t="s">
-        <v>367</v>
+        <v>411</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -6576,10 +6576,10 @@
         <v>26</v>
       </c>
       <c r="E96" t="s">
+        <v>367</v>
+      </c>
+      <c r="F96" t="s">
         <v>368</v>
-      </c>
-      <c r="F96" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -6590,10 +6590,10 @@
         <v>27</v>
       </c>
       <c r="E97" t="s">
+        <v>369</v>
+      </c>
+      <c r="F97" t="s">
         <v>370</v>
-      </c>
-      <c r="F97" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -6604,10 +6604,10 @@
         <v>28</v>
       </c>
       <c r="E98" t="s">
+        <v>371</v>
+      </c>
+      <c r="F98" t="s">
         <v>372</v>
-      </c>
-      <c r="F98" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -6618,10 +6618,10 @@
         <v>29</v>
       </c>
       <c r="E99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F99" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -6632,10 +6632,10 @@
         <v>30</v>
       </c>
       <c r="E100" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F100" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -6646,10 +6646,10 @@
         <v>31</v>
       </c>
       <c r="E101" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F101" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -6660,10 +6660,10 @@
         <v>32</v>
       </c>
       <c r="E102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F102" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -6674,10 +6674,10 @@
         <v>33</v>
       </c>
       <c r="E103" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F103" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix i18n numbers in cards; add unfinished i18n
</commit_message>
<xml_diff>
--- a/tools/data-processing/data.xlsx
+++ b/tools/data-processing/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\might-and-magic\arcomage-hd\tools\data-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E0712D-D634-463A-8BF5-571EA1548225}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A96CEF-ABA0-4282-A0DE-C903AEB8B661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="413">
   <si>
     <t>Type</t>
   </si>
@@ -500,9 +500,6 @@
     <t>+4 Tower, you lose 3 recruits, 2 damage to enemy tower</t>
   </si>
   <si>
-    <t>+8 Tower. This card can't be discarded without playing it</t>
-  </si>
-  <si>
     <t>+1 Magic. +3 Tower. +1 Enemy tower</t>
   </si>
   <si>
@@ -938,9 +935,6 @@
     <t>焚心之火</t>
   </si>
   <si>
-    <t>宝石产量+2，城堡-5</t>
-  </si>
-  <si>
     <t>忠诚代价</t>
   </si>
   <si>
@@ -956,9 +950,6 @@
     <t>神奇翡翠</t>
   </si>
   <si>
-    <t>宝石产量+1，城堡+5</t>
-  </si>
-  <si>
     <t>赌命狂徒</t>
   </si>
   <si>
@@ -980,9 +971,6 @@
     <t>生死相斗</t>
   </si>
   <si>
-    <t>双方宝石产量同时-1，城堡同时-7</t>
-  </si>
-  <si>
     <t>幻火之石</t>
   </si>
   <si>
@@ -1263,6 +1251,21 @@
   </si>
   <si>
     <t>对手宝石-10，砖头-5，你得到其中一半（向上取整）</t>
+  </si>
+  <si>
+    <t>+3 Tower. This card can't be discarded without playing it</t>
+  </si>
+  <si>
+    <t>城堡+5</t>
+  </si>
+  <si>
+    <t>城堡-5，宝石产量+2</t>
+  </si>
+  <si>
+    <t>城堡+5，宝石产量+1</t>
+  </si>
+  <si>
+    <t>双方城堡同时-7，宝石产量同时-1</t>
   </si>
 </sst>
 </file>
@@ -1583,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399247F-B0D6-4509-8DB3-900582E8810F}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1735,7 +1738,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2218,7 +2221,7 @@
         <v>116</v>
       </c>
       <c r="G31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2241,7 +2244,7 @@
         <v>126</v>
       </c>
       <c r="G32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2264,7 +2267,7 @@
         <v>134</v>
       </c>
       <c r="G33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2287,7 +2290,7 @@
         <v>137</v>
       </c>
       <c r="G34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2310,7 +2313,7 @@
         <v>140</v>
       </c>
       <c r="G35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2430,7 +2433,7 @@
         <v>47</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>157</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2470,7 +2473,7 @@
         <v>49</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2570,7 +2573,7 @@
         <v>50</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2610,7 +2613,7 @@
         <v>48</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2630,7 +2633,7 @@
         <v>55</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2650,7 +2653,7 @@
         <v>53</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2670,7 +2673,7 @@
         <v>51</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2690,7 +2693,7 @@
         <v>56</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2710,7 +2713,7 @@
         <v>46</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2730,7 +2733,7 @@
         <v>58</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2770,7 +2773,7 @@
         <v>57</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2790,7 +2793,7 @@
         <v>59</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2810,7 +2813,7 @@
         <v>61</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,7 +2833,7 @@
         <v>60</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2850,7 +2853,7 @@
         <v>62</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2870,7 +2873,7 @@
         <v>63</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2890,7 +2893,7 @@
         <v>54</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2913,7 +2916,7 @@
         <v>143</v>
       </c>
       <c r="G65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2936,7 +2939,7 @@
         <v>144</v>
       </c>
       <c r="G66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2959,7 +2962,7 @@
         <v>156</v>
       </c>
       <c r="G67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2979,10 +2982,10 @@
         <v>100</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -3002,10 +3005,10 @@
         <v>101</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -3025,7 +3028,7 @@
         <v>102</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3045,7 +3048,7 @@
         <v>103</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3065,7 +3068,7 @@
         <v>65</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3085,7 +3088,7 @@
         <v>106</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3125,7 +3128,7 @@
         <v>67</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3145,7 +3148,7 @@
         <v>69</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3165,7 +3168,7 @@
         <v>75</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3185,7 +3188,7 @@
         <v>68</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3205,7 +3208,7 @@
         <v>71</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3225,7 +3228,7 @@
         <v>74</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -3245,7 +3248,7 @@
         <v>109</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -3265,7 +3268,7 @@
         <v>77</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -3285,7 +3288,7 @@
         <v>64</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -3305,7 +3308,7 @@
         <v>70</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -3325,7 +3328,7 @@
         <v>73</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -3345,7 +3348,7 @@
         <v>108</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -3365,7 +3368,7 @@
         <v>72</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -3385,7 +3388,7 @@
         <v>76</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -3405,7 +3408,7 @@
         <v>79</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -3425,7 +3428,7 @@
         <v>81</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -3445,7 +3448,7 @@
         <v>78</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -3465,7 +3468,7 @@
         <v>80</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -3485,7 +3488,7 @@
         <v>83</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -3505,7 +3508,7 @@
         <v>82</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -3545,7 +3548,7 @@
         <v>84</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3565,7 +3568,7 @@
         <v>85</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -3585,7 +3588,7 @@
         <v>86</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -3605,10 +3608,10 @@
         <v>105</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -3628,10 +3631,10 @@
         <v>104</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G100" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -3651,10 +3654,10 @@
         <v>107</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G101" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -3674,10 +3677,10 @@
         <v>110</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G102" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -3697,10 +3700,10 @@
         <v>111</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G103" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3713,8 +3716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C56CEB-8692-4AC2-8CE6-B1BDDA007E98}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3823,7 +3826,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -4162,7 +4165,7 @@
         <v>116</v>
       </c>
       <c r="G31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4179,7 +4182,7 @@
         <v>126</v>
       </c>
       <c r="G32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4196,7 +4199,7 @@
         <v>134</v>
       </c>
       <c r="G33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4213,7 +4216,7 @@
         <v>137</v>
       </c>
       <c r="G34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4230,7 +4233,7 @@
         <v>140</v>
       </c>
       <c r="G35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4314,7 +4317,7 @@
         <v>47</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>157</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4342,7 +4345,7 @@
         <v>49</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4412,7 +4415,7 @@
         <v>50</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -4440,7 +4443,7 @@
         <v>48</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -4454,7 +4457,7 @@
         <v>55</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -4468,7 +4471,7 @@
         <v>53</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -4482,7 +4485,7 @@
         <v>51</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -4496,7 +4499,7 @@
         <v>56</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -4510,7 +4513,7 @@
         <v>46</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -4524,7 +4527,7 @@
         <v>58</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -4552,7 +4555,7 @@
         <v>57</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -4566,7 +4569,7 @@
         <v>59</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -4580,7 +4583,7 @@
         <v>61</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -4594,7 +4597,7 @@
         <v>60</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -4608,7 +4611,7 @@
         <v>62</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -4622,7 +4625,7 @@
         <v>63</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4636,7 +4639,7 @@
         <v>54</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -4653,7 +4656,7 @@
         <v>143</v>
       </c>
       <c r="G65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -4670,7 +4673,7 @@
         <v>144</v>
       </c>
       <c r="G66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -4687,7 +4690,7 @@
         <v>156</v>
       </c>
       <c r="G67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -4701,10 +4704,10 @@
         <v>100</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -4718,10 +4721,10 @@
         <v>101</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -4735,7 +4738,7 @@
         <v>102</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -4749,7 +4752,7 @@
         <v>103</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -4763,7 +4766,7 @@
         <v>65</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -4777,7 +4780,7 @@
         <v>106</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -4805,7 +4808,7 @@
         <v>67</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -4819,7 +4822,7 @@
         <v>69</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -4833,7 +4836,7 @@
         <v>75</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -4847,7 +4850,7 @@
         <v>68</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -4861,7 +4864,7 @@
         <v>71</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -4875,7 +4878,7 @@
         <v>74</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -4889,7 +4892,7 @@
         <v>109</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -4903,7 +4906,7 @@
         <v>77</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -4917,7 +4920,7 @@
         <v>64</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -4931,7 +4934,7 @@
         <v>70</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -4945,7 +4948,7 @@
         <v>73</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -4959,7 +4962,7 @@
         <v>108</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -4973,7 +4976,7 @@
         <v>72</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -4987,7 +4990,7 @@
         <v>76</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -5001,7 +5004,7 @@
         <v>79</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -5015,7 +5018,7 @@
         <v>81</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -5029,7 +5032,7 @@
         <v>78</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -5043,7 +5046,7 @@
         <v>80</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -5057,7 +5060,7 @@
         <v>83</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -5071,7 +5074,7 @@
         <v>82</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -5099,7 +5102,7 @@
         <v>84</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -5113,7 +5116,7 @@
         <v>85</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -5127,7 +5130,7 @@
         <v>86</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -5141,10 +5144,10 @@
         <v>105</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -5158,10 +5161,10 @@
         <v>104</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G100" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -5175,10 +5178,10 @@
         <v>107</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G101" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -5192,10 +5195,10 @@
         <v>110</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G102" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -5209,10 +5212,10 @@
         <v>111</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G103" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -5225,8 +5228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85D8E1A-6405-4E81-99A0-42E9F3DFBBDB}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5260,10 +5263,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" t="s">
         <v>210</v>
-      </c>
-      <c r="F2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5274,10 +5277,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F3" t="s">
         <v>255</v>
-      </c>
-      <c r="F3" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5288,10 +5291,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F4" t="s">
         <v>257</v>
-      </c>
-      <c r="F4" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5302,10 +5305,10 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5" t="s">
         <v>212</v>
-      </c>
-      <c r="F5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5316,10 +5319,10 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F6" t="s">
         <v>214</v>
-      </c>
-      <c r="F6" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5330,10 +5333,10 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -5344,10 +5347,10 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" t="s">
         <v>217</v>
-      </c>
-      <c r="F8" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -5358,10 +5361,10 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
+        <v>218</v>
+      </c>
+      <c r="F9" t="s">
         <v>219</v>
-      </c>
-      <c r="F9" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -5372,10 +5375,10 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" t="s">
         <v>221</v>
-      </c>
-      <c r="F10" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -5386,10 +5389,10 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" t="s">
         <v>223</v>
-      </c>
-      <c r="F11" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -5400,10 +5403,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F12" t="s">
         <v>259</v>
-      </c>
-      <c r="F12" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5414,10 +5417,10 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
+        <v>260</v>
+      </c>
+      <c r="F13" t="s">
         <v>261</v>
-      </c>
-      <c r="F13" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -5428,10 +5431,10 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
+        <v>262</v>
+      </c>
+      <c r="F14" t="s">
         <v>263</v>
-      </c>
-      <c r="F14" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -5442,10 +5445,10 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
+        <v>264</v>
+      </c>
+      <c r="F15" t="s">
         <v>265</v>
-      </c>
-      <c r="F15" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -5456,10 +5459,10 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" t="s">
         <v>267</v>
-      </c>
-      <c r="F16" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -5470,10 +5473,10 @@
         <v>15</v>
       </c>
       <c r="E17" t="s">
+        <v>268</v>
+      </c>
+      <c r="F17" t="s">
         <v>269</v>
-      </c>
-      <c r="F17" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -5484,10 +5487,10 @@
         <v>16</v>
       </c>
       <c r="E18" t="s">
+        <v>270</v>
+      </c>
+      <c r="F18" t="s">
         <v>271</v>
-      </c>
-      <c r="F18" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -5498,10 +5501,10 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
+        <v>272</v>
+      </c>
+      <c r="F19" t="s">
         <v>273</v>
-      </c>
-      <c r="F19" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -5512,10 +5515,10 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
+        <v>274</v>
+      </c>
+      <c r="F20" t="s">
         <v>275</v>
-      </c>
-      <c r="F20" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -5526,10 +5529,10 @@
         <v>19</v>
       </c>
       <c r="E21" t="s">
+        <v>276</v>
+      </c>
+      <c r="F21" t="s">
         <v>277</v>
-      </c>
-      <c r="F21" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -5540,10 +5543,10 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
+        <v>278</v>
+      </c>
+      <c r="F22" t="s">
         <v>279</v>
-      </c>
-      <c r="F22" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -5554,10 +5557,10 @@
         <v>21</v>
       </c>
       <c r="E23" t="s">
+        <v>280</v>
+      </c>
+      <c r="F23" t="s">
         <v>281</v>
-      </c>
-      <c r="F23" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -5568,10 +5571,10 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
+        <v>282</v>
+      </c>
+      <c r="F24" t="s">
         <v>283</v>
-      </c>
-      <c r="F24" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -5582,10 +5585,10 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
+        <v>284</v>
+      </c>
+      <c r="F25" t="s">
         <v>285</v>
-      </c>
-      <c r="F25" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -5596,10 +5599,10 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
+        <v>286</v>
+      </c>
+      <c r="F26" t="s">
         <v>287</v>
-      </c>
-      <c r="F26" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -5610,10 +5613,10 @@
         <v>25</v>
       </c>
       <c r="E27" t="s">
+        <v>288</v>
+      </c>
+      <c r="F27" t="s">
         <v>289</v>
-      </c>
-      <c r="F27" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -5624,10 +5627,10 @@
         <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F28" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -5638,10 +5641,10 @@
         <v>27</v>
       </c>
       <c r="E29" t="s">
+        <v>291</v>
+      </c>
+      <c r="F29" t="s">
         <v>292</v>
-      </c>
-      <c r="F29" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -5652,10 +5655,10 @@
         <v>28</v>
       </c>
       <c r="E30" t="s">
+        <v>293</v>
+      </c>
+      <c r="F30" t="s">
         <v>294</v>
-      </c>
-      <c r="F30" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -5666,10 +5669,10 @@
         <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F31" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -5680,10 +5683,10 @@
         <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F32" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -5694,10 +5697,10 @@
         <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F33" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -5708,10 +5711,10 @@
         <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="F34" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -5722,10 +5725,10 @@
         <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F35" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -5736,10 +5739,10 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
+        <v>295</v>
+      </c>
+      <c r="F36" t="s">
         <v>296</v>
-      </c>
-      <c r="F36" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -5750,10 +5753,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
+        <v>297</v>
+      </c>
+      <c r="F37" t="s">
         <v>298</v>
-      </c>
-      <c r="F37" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -5764,10 +5767,10 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
+        <v>224</v>
+      </c>
+      <c r="F38" t="s">
         <v>225</v>
-      </c>
-      <c r="F38" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -5778,10 +5781,10 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
+        <v>226</v>
+      </c>
+      <c r="F39" t="s">
         <v>227</v>
-      </c>
-      <c r="F39" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -5792,10 +5795,10 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
+        <v>299</v>
+      </c>
+      <c r="F40" t="s">
         <v>300</v>
-      </c>
-      <c r="F40" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -5806,10 +5809,10 @@
         <v>5</v>
       </c>
       <c r="E41" t="s">
+        <v>228</v>
+      </c>
+      <c r="F41" t="s">
         <v>229</v>
-      </c>
-      <c r="F41" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -5820,10 +5823,10 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
+        <v>230</v>
+      </c>
+      <c r="F42" t="s">
         <v>231</v>
-      </c>
-      <c r="F42" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -5834,10 +5837,10 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
+        <v>232</v>
+      </c>
+      <c r="F43" t="s">
         <v>233</v>
-      </c>
-      <c r="F43" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -5848,10 +5851,10 @@
         <v>8</v>
       </c>
       <c r="E44" t="s">
+        <v>234</v>
+      </c>
+      <c r="F44" t="s">
         <v>235</v>
-      </c>
-      <c r="F44" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -5862,10 +5865,10 @@
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F45" t="s">
-        <v>226</v>
+        <v>409</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -5876,10 +5879,10 @@
         <v>10</v>
       </c>
       <c r="E46" t="s">
+        <v>237</v>
+      </c>
+      <c r="F46" t="s">
         <v>238</v>
-      </c>
-      <c r="F46" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -5890,10 +5893,10 @@
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F47" t="s">
-        <v>303</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -5904,10 +5907,10 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F48" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -5918,10 +5921,10 @@
         <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F49" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -5932,10 +5935,10 @@
         <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F50" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -5946,10 +5949,10 @@
         <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F51" t="s">
-        <v>309</v>
+        <v>411</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -5960,10 +5963,10 @@
         <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F52" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -5974,10 +5977,10 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F53" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -5988,10 +5991,10 @@
         <v>18</v>
       </c>
       <c r="E54" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F54" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -6002,10 +6005,10 @@
         <v>19</v>
       </c>
       <c r="E55" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F55" t="s">
-        <v>317</v>
+        <v>412</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -6016,10 +6019,10 @@
         <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F56" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -6030,10 +6033,10 @@
         <v>21</v>
       </c>
       <c r="E57" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F57" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -6044,10 +6047,10 @@
         <v>22</v>
       </c>
       <c r="E58" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F58" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -6058,10 +6061,10 @@
         <v>23</v>
       </c>
       <c r="E59" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F59" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -6072,10 +6075,10 @@
         <v>24</v>
       </c>
       <c r="E60" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F60" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -6086,10 +6089,10 @@
         <v>25</v>
       </c>
       <c r="E61" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F61" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -6100,10 +6103,10 @@
         <v>26</v>
       </c>
       <c r="E62" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F62" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -6114,10 +6117,10 @@
         <v>27</v>
       </c>
       <c r="E63" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F63" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -6128,10 +6131,10 @@
         <v>28</v>
       </c>
       <c r="E64" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F64" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -6142,10 +6145,10 @@
         <v>29</v>
       </c>
       <c r="E65" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F65" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -6156,10 +6159,10 @@
         <v>30</v>
       </c>
       <c r="E66" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F66" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -6170,10 +6173,10 @@
         <v>31</v>
       </c>
       <c r="E67" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F67" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -6184,10 +6187,10 @@
         <v>32</v>
       </c>
       <c r="E68" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F68" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -6198,10 +6201,10 @@
         <v>33</v>
       </c>
       <c r="E69" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F69" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -6212,10 +6215,10 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
+        <v>239</v>
+      </c>
+      <c r="F70" t="s">
         <v>240</v>
-      </c>
-      <c r="F70" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -6226,10 +6229,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F71" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -6240,10 +6243,10 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
+        <v>241</v>
+      </c>
+      <c r="F72" t="s">
         <v>242</v>
-      </c>
-      <c r="F72" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -6254,10 +6257,10 @@
         <v>3</v>
       </c>
       <c r="E73" t="s">
+        <v>243</v>
+      </c>
+      <c r="F73" t="s">
         <v>244</v>
-      </c>
-      <c r="F73" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -6268,10 +6271,10 @@
         <v>4</v>
       </c>
       <c r="E74" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F74" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -6282,10 +6285,10 @@
         <v>5</v>
       </c>
       <c r="E75" t="s">
+        <v>245</v>
+      </c>
+      <c r="F75" t="s">
         <v>246</v>
-      </c>
-      <c r="F75" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -6296,10 +6299,10 @@
         <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F76" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -6310,10 +6313,10 @@
         <v>7</v>
       </c>
       <c r="E77" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F77" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -6324,10 +6327,10 @@
         <v>8</v>
       </c>
       <c r="E78" t="s">
+        <v>248</v>
+      </c>
+      <c r="F78" t="s">
         <v>249</v>
-      </c>
-      <c r="F78" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -6338,10 +6341,10 @@
         <v>9</v>
       </c>
       <c r="E79" t="s">
+        <v>250</v>
+      </c>
+      <c r="F79" t="s">
         <v>251</v>
-      </c>
-      <c r="F79" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -6352,10 +6355,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
+        <v>252</v>
+      </c>
+      <c r="F80" t="s">
         <v>253</v>
-      </c>
-      <c r="F80" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -6366,10 +6369,10 @@
         <v>11</v>
       </c>
       <c r="E81" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F81" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -6380,10 +6383,10 @@
         <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F82" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -6394,10 +6397,10 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F83" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -6408,10 +6411,10 @@
         <v>14</v>
       </c>
       <c r="E84" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F84" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -6422,10 +6425,10 @@
         <v>15</v>
       </c>
       <c r="E85" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F85" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -6436,10 +6439,10 @@
         <v>16</v>
       </c>
       <c r="E86" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F86" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -6450,10 +6453,10 @@
         <v>17</v>
       </c>
       <c r="E87" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F87" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -6464,10 +6467,10 @@
         <v>18</v>
       </c>
       <c r="E88" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F88" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -6478,10 +6481,10 @@
         <v>19</v>
       </c>
       <c r="E89" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F89" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -6492,10 +6495,10 @@
         <v>20</v>
       </c>
       <c r="E90" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F90" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -6506,10 +6509,10 @@
         <v>21</v>
       </c>
       <c r="E91" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F91" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -6520,10 +6523,10 @@
         <v>22</v>
       </c>
       <c r="E92" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F92" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -6534,10 +6537,10 @@
         <v>23</v>
       </c>
       <c r="E93" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F93" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -6548,10 +6551,10 @@
         <v>24</v>
       </c>
       <c r="E94" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F94" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -6562,10 +6565,10 @@
         <v>25</v>
       </c>
       <c r="E95" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F95" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -6576,10 +6579,10 @@
         <v>26</v>
       </c>
       <c r="E96" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F96" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -6590,10 +6593,10 @@
         <v>27</v>
       </c>
       <c r="E97" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F97" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -6604,10 +6607,10 @@
         <v>28</v>
       </c>
       <c r="E98" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F98" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -6618,10 +6621,10 @@
         <v>29</v>
       </c>
       <c r="E99" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F99" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -6632,10 +6635,10 @@
         <v>30</v>
       </c>
       <c r="E100" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="F100" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -6646,10 +6649,10 @@
         <v>31</v>
       </c>
       <c r="E101" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F101" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -6660,10 +6663,10 @@
         <v>32</v>
       </c>
       <c r="E102" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="F102" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -6674,10 +6677,10 @@
         <v>33</v>
       </c>
       <c r="E103" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F103" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: init action; settings states
</commit_message>
<xml_diff>
--- a/tools/data-processing/data.xlsx
+++ b/tools/data-processing/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\might-and-magic\arcomage-hd\tools\data-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A96CEF-ABA0-4282-A0DE-C903AEB8B661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0027328C-4658-4B81-83C8-0CFF1BA54288}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="4" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
@@ -1266,6 +1263,9 @@
   </si>
   <si>
     <t>双方城堡同时-7，宝石产量同时-1</t>
+  </si>
+  <si>
+    <t>Prob</t>
   </si>
 </sst>
 </file>
@@ -1586,15 +1586,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399247F-B0D6-4509-8DB3-900582E8810F}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="58.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1606,19 +1606,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>412</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1635,10 +1635,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1655,10 +1655,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1675,10 +1675,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1695,10 +1695,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1715,10 +1715,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1735,10 +1735,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1755,10 +1755,10 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1775,10 +1775,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1795,10 +1795,10 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1815,10 +1815,10 @@
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1835,10 +1835,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1855,10 +1855,10 @@
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1875,10 +1875,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1895,10 +1895,10 @@
         <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1915,10 +1915,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1935,10 +1935,10 @@
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1955,10 +1955,10 @@
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1975,10 +1975,10 @@
         <v>6</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1995,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2015,10 +2015,10 @@
         <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2035,10 +2035,10 @@
         <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2055,10 +2055,10 @@
         <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2075,10 +2075,10 @@
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2095,10 +2095,10 @@
         <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2115,10 +2115,10 @@
         <v>15</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2135,10 +2135,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2155,10 +2155,10 @@
         <v>18</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -2175,10 +2175,10 @@
         <v>24</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -2195,10 +2195,10 @@
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2215,13 +2215,13 @@
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2238,13 +2238,13 @@
         <v>6</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2261,13 +2261,13 @@
         <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2284,13 +2284,13 @@
         <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2307,13 +2307,13 @@
         <v>17</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2330,10 +2330,10 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2350,10 +2350,10 @@
         <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2370,10 +2370,10 @@
         <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2390,10 +2390,10 @@
         <v>3</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2410,10 +2410,10 @@
         <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2430,10 +2430,10 @@
         <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2450,10 +2450,10 @@
         <v>4</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2470,10 +2470,10 @@
         <v>6</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2490,10 +2490,10 @@
         <v>2</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2510,10 +2510,10 @@
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2530,10 +2530,10 @@
         <v>4</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2550,10 +2550,10 @@
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2570,10 +2570,10 @@
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2590,10 +2590,10 @@
         <v>7</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2610,10 +2610,10 @@
         <v>6</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2630,10 +2630,10 @@
         <v>9</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2650,10 +2650,10 @@
         <v>8</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2670,10 +2670,10 @@
         <v>7</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2690,10 +2690,10 @@
         <v>10</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2710,10 +2710,10 @@
         <v>5</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2730,10 +2730,10 @@
         <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2750,10 +2750,10 @@
         <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2770,10 +2770,10 @@
         <v>12</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2790,10 +2790,10 @@
         <v>14</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2810,10 +2810,10 @@
         <v>16</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,10 +2830,10 @@
         <v>15</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2850,10 +2850,10 @@
         <v>17</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2870,10 +2870,10 @@
         <v>21</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2890,10 +2890,10 @@
         <v>8</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2910,13 +2910,13 @@
         <v>0</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2933,13 +2933,13 @@
         <v>0</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2956,13 +2956,13 @@
         <v>5</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2979,13 +2979,13 @@
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -3002,13 +3002,13 @@
         <v>18</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -3025,10 +3025,10 @@
         <v>0</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3045,10 +3045,10 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3065,10 +3065,10 @@
         <v>1</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3085,10 +3085,10 @@
         <v>3</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3105,10 +3105,10 @@
         <v>2</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3125,10 +3125,10 @@
         <v>3</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3145,10 +3145,10 @@
         <v>4</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3165,10 +3165,10 @@
         <v>6</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3185,10 +3185,10 @@
         <v>3</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3205,10 +3205,10 @@
         <v>5</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3225,10 +3225,10 @@
         <v>6</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -3245,10 +3245,10 @@
         <v>7</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -3265,10 +3265,10 @@
         <v>8</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -3285,10 +3285,10 @@
         <v>0</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -3305,10 +3305,10 @@
         <v>5</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -3325,10 +3325,10 @@
         <v>6</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -3345,10 +3345,10 @@
         <v>6</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -3365,10 +3365,10 @@
         <v>5</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -3385,10 +3385,10 @@
         <v>8</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -3405,10 +3405,10 @@
         <v>9</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -3425,10 +3425,10 @@
         <v>11</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -3445,10 +3445,10 @@
         <v>9</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -3465,10 +3465,10 @@
         <v>10</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -3485,10 +3485,10 @@
         <v>14</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -3505,10 +3505,10 @@
         <v>11</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -3525,10 +3525,10 @@
         <v>12</v>
       </c>
       <c r="E95" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -3545,10 +3545,10 @@
         <v>15</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3565,10 +3565,10 @@
         <v>17</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -3585,10 +3585,10 @@
         <v>25</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -3605,13 +3605,13 @@
         <v>2</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -3628,13 +3628,13 @@
         <v>2</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G100" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -3651,13 +3651,13 @@
         <v>4</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -3674,13 +3674,13 @@
         <v>13</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G102" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -3697,13 +3697,13 @@
         <v>18</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G103" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3736,13 +3736,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3753,10 +3753,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3767,10 +3767,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3781,10 +3781,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3795,10 +3795,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3809,10 +3809,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -3823,10 +3823,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -3837,10 +3837,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3851,10 +3851,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3865,10 +3865,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3879,10 +3879,10 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3893,10 +3893,10 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -3907,10 +3907,10 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3921,10 +3921,10 @@
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3935,10 +3935,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -3949,10 +3949,10 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3963,10 +3963,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3977,10 +3977,10 @@
         <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3991,10 +3991,10 @@
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -4005,10 +4005,10 @@
         <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -4019,10 +4019,10 @@
         <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -4033,10 +4033,10 @@
         <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -4047,10 +4047,10 @@
         <v>21</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -4061,10 +4061,10 @@
         <v>22</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4075,10 +4075,10 @@
         <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -4089,10 +4089,10 @@
         <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4103,10 +4103,10 @@
         <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -4117,10 +4117,10 @@
         <v>26</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -4131,10 +4131,10 @@
         <v>27</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4145,10 +4145,10 @@
         <v>28</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4159,13 +4159,13 @@
         <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4176,13 +4176,13 @@
         <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4193,13 +4193,13 @@
         <v>31</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4210,13 +4210,13 @@
         <v>32</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4227,13 +4227,13 @@
         <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4244,10 +4244,10 @@
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4258,10 +4258,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4272,10 +4272,10 @@
         <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4286,10 +4286,10 @@
         <v>3</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4300,10 +4300,10 @@
         <v>4</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4314,10 +4314,10 @@
         <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4328,10 +4328,10 @@
         <v>6</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4342,10 +4342,10 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4356,10 +4356,10 @@
         <v>8</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -4370,10 +4370,10 @@
         <v>9</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4384,10 +4384,10 @@
         <v>10</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -4398,10 +4398,10 @@
         <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4412,10 +4412,10 @@
         <v>12</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -4426,10 +4426,10 @@
         <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -4440,10 +4440,10 @@
         <v>14</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -4454,10 +4454,10 @@
         <v>15</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -4468,10 +4468,10 @@
         <v>16</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -4482,10 +4482,10 @@
         <v>17</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -4496,10 +4496,10 @@
         <v>18</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -4510,10 +4510,10 @@
         <v>19</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -4524,10 +4524,10 @@
         <v>20</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -4538,10 +4538,10 @@
         <v>21</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -4552,10 +4552,10 @@
         <v>22</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -4566,10 +4566,10 @@
         <v>23</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -4580,10 +4580,10 @@
         <v>24</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -4594,10 +4594,10 @@
         <v>25</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -4608,10 +4608,10 @@
         <v>26</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -4622,10 +4622,10 @@
         <v>27</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4636,10 +4636,10 @@
         <v>28</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -4650,13 +4650,13 @@
         <v>29</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -4667,13 +4667,13 @@
         <v>30</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -4684,13 +4684,13 @@
         <v>31</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -4701,13 +4701,13 @@
         <v>32</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -4718,13 +4718,13 @@
         <v>33</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -4735,10 +4735,10 @@
         <v>0</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -4749,10 +4749,10 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -4763,10 +4763,10 @@
         <v>2</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -4777,10 +4777,10 @@
         <v>3</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -4791,10 +4791,10 @@
         <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -4805,10 +4805,10 @@
         <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -4819,10 +4819,10 @@
         <v>6</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -4833,10 +4833,10 @@
         <v>7</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -4847,10 +4847,10 @@
         <v>8</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -4861,10 +4861,10 @@
         <v>9</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -4875,10 +4875,10 @@
         <v>10</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -4889,10 +4889,10 @@
         <v>11</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -4903,10 +4903,10 @@
         <v>12</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -4917,10 +4917,10 @@
         <v>13</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -4931,10 +4931,10 @@
         <v>14</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -4945,10 +4945,10 @@
         <v>15</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -4959,10 +4959,10 @@
         <v>16</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -4973,10 +4973,10 @@
         <v>17</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -4987,10 +4987,10 @@
         <v>18</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -5001,10 +5001,10 @@
         <v>19</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -5015,10 +5015,10 @@
         <v>20</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -5029,10 +5029,10 @@
         <v>21</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -5043,10 +5043,10 @@
         <v>22</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -5057,10 +5057,10 @@
         <v>23</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -5071,10 +5071,10 @@
         <v>24</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -5085,10 +5085,10 @@
         <v>25</v>
       </c>
       <c r="E95" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -5099,10 +5099,10 @@
         <v>26</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -5113,10 +5113,10 @@
         <v>27</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -5127,10 +5127,10 @@
         <v>28</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -5141,13 +5141,13 @@
         <v>29</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -5158,13 +5158,13 @@
         <v>30</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G100" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -5175,13 +5175,13 @@
         <v>31</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -5192,13 +5192,13 @@
         <v>32</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G102" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -5209,13 +5209,13 @@
         <v>33</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G103" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5228,7 +5228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85D8E1A-6405-4E81-99A0-42E9F3DFBBDB}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
@@ -5246,13 +5246,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -5263,10 +5263,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" t="s">
         <v>209</v>
-      </c>
-      <c r="F2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5277,10 +5277,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" t="s">
         <v>254</v>
-      </c>
-      <c r="F3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5291,10 +5291,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F4" t="s">
         <v>256</v>
-      </c>
-      <c r="F4" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5305,10 +5305,10 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" t="s">
         <v>211</v>
-      </c>
-      <c r="F5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5319,10 +5319,10 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" t="s">
         <v>213</v>
-      </c>
-      <c r="F6" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5333,10 +5333,10 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -5347,10 +5347,10 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" t="s">
         <v>216</v>
-      </c>
-      <c r="F8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -5361,10 +5361,10 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" t="s">
         <v>218</v>
-      </c>
-      <c r="F9" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -5375,10 +5375,10 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" t="s">
         <v>220</v>
-      </c>
-      <c r="F10" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -5389,10 +5389,10 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" t="s">
         <v>222</v>
-      </c>
-      <c r="F11" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -5403,10 +5403,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F12" t="s">
         <v>258</v>
-      </c>
-      <c r="F12" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5417,10 +5417,10 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" t="s">
         <v>260</v>
-      </c>
-      <c r="F13" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -5431,10 +5431,10 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
+        <v>261</v>
+      </c>
+      <c r="F14" t="s">
         <v>262</v>
-      </c>
-      <c r="F14" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -5445,10 +5445,10 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F15" t="s">
         <v>264</v>
-      </c>
-      <c r="F15" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -5459,10 +5459,10 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F16" t="s">
         <v>266</v>
-      </c>
-      <c r="F16" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -5473,10 +5473,10 @@
         <v>15</v>
       </c>
       <c r="E17" t="s">
+        <v>267</v>
+      </c>
+      <c r="F17" t="s">
         <v>268</v>
-      </c>
-      <c r="F17" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -5487,10 +5487,10 @@
         <v>16</v>
       </c>
       <c r="E18" t="s">
+        <v>269</v>
+      </c>
+      <c r="F18" t="s">
         <v>270</v>
-      </c>
-      <c r="F18" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -5501,10 +5501,10 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
+        <v>271</v>
+      </c>
+      <c r="F19" t="s">
         <v>272</v>
-      </c>
-      <c r="F19" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -5515,10 +5515,10 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
+        <v>273</v>
+      </c>
+      <c r="F20" t="s">
         <v>274</v>
-      </c>
-      <c r="F20" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -5529,10 +5529,10 @@
         <v>19</v>
       </c>
       <c r="E21" t="s">
+        <v>275</v>
+      </c>
+      <c r="F21" t="s">
         <v>276</v>
-      </c>
-      <c r="F21" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -5543,10 +5543,10 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22" t="s">
         <v>278</v>
-      </c>
-      <c r="F22" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -5557,10 +5557,10 @@
         <v>21</v>
       </c>
       <c r="E23" t="s">
+        <v>279</v>
+      </c>
+      <c r="F23" t="s">
         <v>280</v>
-      </c>
-      <c r="F23" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -5571,10 +5571,10 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
+        <v>281</v>
+      </c>
+      <c r="F24" t="s">
         <v>282</v>
-      </c>
-      <c r="F24" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -5585,10 +5585,10 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
+        <v>283</v>
+      </c>
+      <c r="F25" t="s">
         <v>284</v>
-      </c>
-      <c r="F25" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -5599,10 +5599,10 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
+        <v>285</v>
+      </c>
+      <c r="F26" t="s">
         <v>286</v>
-      </c>
-      <c r="F26" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -5613,10 +5613,10 @@
         <v>25</v>
       </c>
       <c r="E27" t="s">
+        <v>287</v>
+      </c>
+      <c r="F27" t="s">
         <v>288</v>
-      </c>
-      <c r="F27" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -5627,10 +5627,10 @@
         <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -5641,10 +5641,10 @@
         <v>27</v>
       </c>
       <c r="E29" t="s">
+        <v>290</v>
+      </c>
+      <c r="F29" t="s">
         <v>291</v>
-      </c>
-      <c r="F29" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -5655,10 +5655,10 @@
         <v>28</v>
       </c>
       <c r="E30" t="s">
+        <v>292</v>
+      </c>
+      <c r="F30" t="s">
         <v>293</v>
-      </c>
-      <c r="F30" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -5669,10 +5669,10 @@
         <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -5683,10 +5683,10 @@
         <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F32" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -5697,10 +5697,10 @@
         <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F33" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -5711,10 +5711,10 @@
         <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F34" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -5725,10 +5725,10 @@
         <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F35" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -5739,10 +5739,10 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
+        <v>294</v>
+      </c>
+      <c r="F36" t="s">
         <v>295</v>
-      </c>
-      <c r="F36" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -5753,10 +5753,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
+        <v>296</v>
+      </c>
+      <c r="F37" t="s">
         <v>297</v>
-      </c>
-      <c r="F37" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -5767,10 +5767,10 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
+        <v>223</v>
+      </c>
+      <c r="F38" t="s">
         <v>224</v>
-      </c>
-      <c r="F38" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -5781,10 +5781,10 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
+        <v>225</v>
+      </c>
+      <c r="F39" t="s">
         <v>226</v>
-      </c>
-      <c r="F39" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -5795,10 +5795,10 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
+        <v>298</v>
+      </c>
+      <c r="F40" t="s">
         <v>299</v>
-      </c>
-      <c r="F40" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -5809,10 +5809,10 @@
         <v>5</v>
       </c>
       <c r="E41" t="s">
+        <v>227</v>
+      </c>
+      <c r="F41" t="s">
         <v>228</v>
-      </c>
-      <c r="F41" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -5823,10 +5823,10 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" t="s">
         <v>230</v>
-      </c>
-      <c r="F42" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -5837,10 +5837,10 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
+        <v>231</v>
+      </c>
+      <c r="F43" t="s">
         <v>232</v>
-      </c>
-      <c r="F43" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -5851,10 +5851,10 @@
         <v>8</v>
       </c>
       <c r="E44" t="s">
+        <v>233</v>
+      </c>
+      <c r="F44" t="s">
         <v>234</v>
-      </c>
-      <c r="F44" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -5865,10 +5865,10 @@
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F45" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -5879,10 +5879,10 @@
         <v>10</v>
       </c>
       <c r="E46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F46" t="s">
         <v>237</v>
-      </c>
-      <c r="F46" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -5893,10 +5893,10 @@
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F47" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -5907,10 +5907,10 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
+        <v>301</v>
+      </c>
+      <c r="F48" t="s">
         <v>302</v>
-      </c>
-      <c r="F48" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -5921,10 +5921,10 @@
         <v>13</v>
       </c>
       <c r="E49" t="s">
+        <v>303</v>
+      </c>
+      <c r="F49" t="s">
         <v>304</v>
-      </c>
-      <c r="F49" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -5935,10 +5935,10 @@
         <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F50" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -5949,10 +5949,10 @@
         <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -5963,10 +5963,10 @@
         <v>16</v>
       </c>
       <c r="E52" t="s">
+        <v>306</v>
+      </c>
+      <c r="F52" t="s">
         <v>307</v>
-      </c>
-      <c r="F52" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -5977,10 +5977,10 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
+        <v>308</v>
+      </c>
+      <c r="F53" t="s">
         <v>309</v>
-      </c>
-      <c r="F53" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -5991,10 +5991,10 @@
         <v>18</v>
       </c>
       <c r="E54" t="s">
+        <v>310</v>
+      </c>
+      <c r="F54" t="s">
         <v>311</v>
-      </c>
-      <c r="F54" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -6005,10 +6005,10 @@
         <v>19</v>
       </c>
       <c r="E55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F55" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -6019,10 +6019,10 @@
         <v>20</v>
       </c>
       <c r="E56" t="s">
+        <v>313</v>
+      </c>
+      <c r="F56" t="s">
         <v>314</v>
-      </c>
-      <c r="F56" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -6033,10 +6033,10 @@
         <v>21</v>
       </c>
       <c r="E57" t="s">
+        <v>315</v>
+      </c>
+      <c r="F57" t="s">
         <v>316</v>
-      </c>
-      <c r="F57" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -6047,10 +6047,10 @@
         <v>22</v>
       </c>
       <c r="E58" t="s">
+        <v>317</v>
+      </c>
+      <c r="F58" t="s">
         <v>318</v>
-      </c>
-      <c r="F58" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -6061,10 +6061,10 @@
         <v>23</v>
       </c>
       <c r="E59" t="s">
+        <v>319</v>
+      </c>
+      <c r="F59" t="s">
         <v>320</v>
-      </c>
-      <c r="F59" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -6075,10 +6075,10 @@
         <v>24</v>
       </c>
       <c r="E60" t="s">
+        <v>321</v>
+      </c>
+      <c r="F60" t="s">
         <v>322</v>
-      </c>
-      <c r="F60" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -6089,10 +6089,10 @@
         <v>25</v>
       </c>
       <c r="E61" t="s">
+        <v>323</v>
+      </c>
+      <c r="F61" t="s">
         <v>324</v>
-      </c>
-      <c r="F61" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -6103,10 +6103,10 @@
         <v>26</v>
       </c>
       <c r="E62" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F62" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -6117,10 +6117,10 @@
         <v>27</v>
       </c>
       <c r="E63" t="s">
+        <v>326</v>
+      </c>
+      <c r="F63" t="s">
         <v>327</v>
-      </c>
-      <c r="F63" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -6131,10 +6131,10 @@
         <v>28</v>
       </c>
       <c r="E64" t="s">
+        <v>328</v>
+      </c>
+      <c r="F64" t="s">
         <v>329</v>
-      </c>
-      <c r="F64" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -6145,10 +6145,10 @@
         <v>29</v>
       </c>
       <c r="E65" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -6159,10 +6159,10 @@
         <v>30</v>
       </c>
       <c r="E66" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F66" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -6173,10 +6173,10 @@
         <v>31</v>
       </c>
       <c r="E67" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F67" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -6187,10 +6187,10 @@
         <v>32</v>
       </c>
       <c r="E68" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F68" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -6201,10 +6201,10 @@
         <v>33</v>
       </c>
       <c r="E69" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F69" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -6215,10 +6215,10 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
+        <v>238</v>
+      </c>
+      <c r="F70" t="s">
         <v>239</v>
-      </c>
-      <c r="F70" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -6229,10 +6229,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
+        <v>330</v>
+      </c>
+      <c r="F71" t="s">
         <v>331</v>
-      </c>
-      <c r="F71" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -6243,10 +6243,10 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
+        <v>240</v>
+      </c>
+      <c r="F72" t="s">
         <v>241</v>
-      </c>
-      <c r="F72" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -6257,10 +6257,10 @@
         <v>3</v>
       </c>
       <c r="E73" t="s">
+        <v>242</v>
+      </c>
+      <c r="F73" t="s">
         <v>243</v>
-      </c>
-      <c r="F73" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -6271,10 +6271,10 @@
         <v>4</v>
       </c>
       <c r="E74" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F74" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -6285,10 +6285,10 @@
         <v>5</v>
       </c>
       <c r="E75" t="s">
+        <v>244</v>
+      </c>
+      <c r="F75" t="s">
         <v>245</v>
-      </c>
-      <c r="F75" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -6299,10 +6299,10 @@
         <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F76" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -6313,10 +6313,10 @@
         <v>7</v>
       </c>
       <c r="E77" t="s">
+        <v>333</v>
+      </c>
+      <c r="F77" t="s">
         <v>334</v>
-      </c>
-      <c r="F77" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -6327,10 +6327,10 @@
         <v>8</v>
       </c>
       <c r="E78" t="s">
+        <v>247</v>
+      </c>
+      <c r="F78" t="s">
         <v>248</v>
-      </c>
-      <c r="F78" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -6341,10 +6341,10 @@
         <v>9</v>
       </c>
       <c r="E79" t="s">
+        <v>249</v>
+      </c>
+      <c r="F79" t="s">
         <v>250</v>
-      </c>
-      <c r="F79" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -6355,10 +6355,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
+        <v>251</v>
+      </c>
+      <c r="F80" t="s">
         <v>252</v>
-      </c>
-      <c r="F80" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -6369,10 +6369,10 @@
         <v>11</v>
       </c>
       <c r="E81" t="s">
+        <v>335</v>
+      </c>
+      <c r="F81" t="s">
         <v>336</v>
-      </c>
-      <c r="F81" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -6383,10 +6383,10 @@
         <v>12</v>
       </c>
       <c r="E82" t="s">
+        <v>337</v>
+      </c>
+      <c r="F82" t="s">
         <v>338</v>
-      </c>
-      <c r="F82" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -6397,10 +6397,10 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
+        <v>339</v>
+      </c>
+      <c r="F83" t="s">
         <v>340</v>
-      </c>
-      <c r="F83" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -6411,10 +6411,10 @@
         <v>14</v>
       </c>
       <c r="E84" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F84" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -6425,10 +6425,10 @@
         <v>15</v>
       </c>
       <c r="E85" t="s">
+        <v>342</v>
+      </c>
+      <c r="F85" t="s">
         <v>343</v>
-      </c>
-      <c r="F85" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -6439,10 +6439,10 @@
         <v>16</v>
       </c>
       <c r="E86" t="s">
+        <v>344</v>
+      </c>
+      <c r="F86" t="s">
         <v>345</v>
-      </c>
-      <c r="F86" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -6453,10 +6453,10 @@
         <v>17</v>
       </c>
       <c r="E87" t="s">
+        <v>346</v>
+      </c>
+      <c r="F87" t="s">
         <v>347</v>
-      </c>
-      <c r="F87" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -6467,10 +6467,10 @@
         <v>18</v>
       </c>
       <c r="E88" t="s">
+        <v>348</v>
+      </c>
+      <c r="F88" t="s">
         <v>349</v>
-      </c>
-      <c r="F88" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -6481,10 +6481,10 @@
         <v>19</v>
       </c>
       <c r="E89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F89" t="s">
         <v>351</v>
-      </c>
-      <c r="F89" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -6495,10 +6495,10 @@
         <v>20</v>
       </c>
       <c r="E90" t="s">
+        <v>352</v>
+      </c>
+      <c r="F90" t="s">
         <v>353</v>
-      </c>
-      <c r="F90" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -6509,10 +6509,10 @@
         <v>21</v>
       </c>
       <c r="E91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F91" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -6523,10 +6523,10 @@
         <v>22</v>
       </c>
       <c r="E92" t="s">
+        <v>355</v>
+      </c>
+      <c r="F92" t="s">
         <v>356</v>
-      </c>
-      <c r="F92" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -6537,10 +6537,10 @@
         <v>23</v>
       </c>
       <c r="E93" t="s">
+        <v>357</v>
+      </c>
+      <c r="F93" t="s">
         <v>358</v>
-      </c>
-      <c r="F93" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -6551,10 +6551,10 @@
         <v>24</v>
       </c>
       <c r="E94" t="s">
+        <v>359</v>
+      </c>
+      <c r="F94" t="s">
         <v>360</v>
-      </c>
-      <c r="F94" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -6565,10 +6565,10 @@
         <v>25</v>
       </c>
       <c r="E95" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F95" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -6579,10 +6579,10 @@
         <v>26</v>
       </c>
       <c r="E96" t="s">
+        <v>362</v>
+      </c>
+      <c r="F96" t="s">
         <v>363</v>
-      </c>
-      <c r="F96" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -6593,10 +6593,10 @@
         <v>27</v>
       </c>
       <c r="E97" t="s">
+        <v>364</v>
+      </c>
+      <c r="F97" t="s">
         <v>365</v>
-      </c>
-      <c r="F97" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -6607,10 +6607,10 @@
         <v>28</v>
       </c>
       <c r="E98" t="s">
+        <v>366</v>
+      </c>
+      <c r="F98" t="s">
         <v>367</v>
-      </c>
-      <c r="F98" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -6621,10 +6621,10 @@
         <v>29</v>
       </c>
       <c r="E99" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F99" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -6635,10 +6635,10 @@
         <v>30</v>
       </c>
       <c r="E100" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F100" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -6649,10 +6649,10 @@
         <v>31</v>
       </c>
       <c r="E101" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -6663,10 +6663,10 @@
         <v>32</v>
       </c>
       <c r="E102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -6677,10 +6677,10 @@
         <v>33</v>
       </c>
       <c r="E103" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F103" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: AI; keyboard shortcut; helmet
</commit_message>
<xml_diff>
--- a/tools/data-processing/data.xlsx
+++ b/tools/data-processing/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\might-and-magic\arcomage-hd\tools\data-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0027328C-4658-4B81-83C8-0CFF1BA54288}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA902BF-CFBD-497A-BB97-3BFFBD629D38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,9 +521,6 @@
     <t>+11 Tower</t>
   </si>
   <si>
-    <t>If Tower &lt; enemy wall, 8 damage to enemy tower. Else 8 damage</t>
-  </si>
-  <si>
     <t>+8 Tower. +3 Wall</t>
   </si>
   <si>
@@ -1266,6 +1263,9 @@
   </si>
   <si>
     <t>Prob</t>
+  </si>
+  <si>
+    <t>If Tower &gt; enemy wall, 8 damage to enemy tower. Else 8 damage</t>
   </si>
 </sst>
 </file>
@@ -1586,9 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399247F-B0D6-4509-8DB3-900582E8810F}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1609,7 +1607,7 @@
         <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1738,7 +1736,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,7 +2219,7 @@
         <v>115</v>
       </c>
       <c r="G31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2244,7 +2242,7 @@
         <v>125</v>
       </c>
       <c r="G32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2267,7 +2265,7 @@
         <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2290,7 +2288,7 @@
         <v>136</v>
       </c>
       <c r="G34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2313,7 +2311,7 @@
         <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2433,7 +2431,7 @@
         <v>46</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2713,7 +2711,7 @@
         <v>45</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2733,7 +2731,7 @@
         <v>57</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2773,7 +2771,7 @@
         <v>56</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2793,7 +2791,7 @@
         <v>58</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2813,7 +2811,7 @@
         <v>60</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2833,7 +2831,7 @@
         <v>59</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2853,7 +2851,7 @@
         <v>61</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2873,7 +2871,7 @@
         <v>62</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2916,7 +2914,7 @@
         <v>142</v>
       </c>
       <c r="G65" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2939,7 +2937,7 @@
         <v>143</v>
       </c>
       <c r="G66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2962,7 +2960,7 @@
         <v>155</v>
       </c>
       <c r="G67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2982,10 +2980,10 @@
         <v>99</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>164</v>
+        <v>412</v>
       </c>
       <c r="G68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -3005,10 +3003,10 @@
         <v>100</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G69" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -3028,7 +3026,7 @@
         <v>101</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3048,7 +3046,7 @@
         <v>102</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -3068,7 +3066,7 @@
         <v>64</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3088,7 +3086,7 @@
         <v>105</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3128,7 +3126,7 @@
         <v>66</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3148,7 +3146,7 @@
         <v>68</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3168,7 +3166,7 @@
         <v>74</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3188,7 +3186,7 @@
         <v>67</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3208,7 +3206,7 @@
         <v>70</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3228,7 +3226,7 @@
         <v>73</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -3248,7 +3246,7 @@
         <v>108</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -3268,7 +3266,7 @@
         <v>76</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -3288,7 +3286,7 @@
         <v>63</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -3308,7 +3306,7 @@
         <v>69</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -3328,7 +3326,7 @@
         <v>72</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -3348,7 +3346,7 @@
         <v>107</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -3368,7 +3366,7 @@
         <v>71</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -3388,7 +3386,7 @@
         <v>75</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -3408,7 +3406,7 @@
         <v>78</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -3428,7 +3426,7 @@
         <v>80</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -3448,7 +3446,7 @@
         <v>77</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -3468,7 +3466,7 @@
         <v>79</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -3488,7 +3486,7 @@
         <v>82</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -3508,7 +3506,7 @@
         <v>81</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -3548,7 +3546,7 @@
         <v>83</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3568,7 +3566,7 @@
         <v>84</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -3588,7 +3586,7 @@
         <v>85</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -3608,10 +3606,10 @@
         <v>104</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G99" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -3631,10 +3629,10 @@
         <v>103</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G100" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -3654,10 +3652,10 @@
         <v>106</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G101" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -3677,10 +3675,10 @@
         <v>109</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G102" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -3700,10 +3698,10 @@
         <v>110</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G103" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3716,9 +3714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C56CEB-8692-4AC2-8CE6-B1BDDA007E98}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3826,7 +3822,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -4165,7 +4161,7 @@
         <v>115</v>
       </c>
       <c r="G31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4182,7 +4178,7 @@
         <v>125</v>
       </c>
       <c r="G32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4199,7 +4195,7 @@
         <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4216,7 +4212,7 @@
         <v>136</v>
       </c>
       <c r="G34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4233,7 +4229,7 @@
         <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4317,7 +4313,7 @@
         <v>46</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4513,7 +4509,7 @@
         <v>45</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -4527,7 +4523,7 @@
         <v>57</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -4555,7 +4551,7 @@
         <v>56</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -4569,7 +4565,7 @@
         <v>58</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -4583,7 +4579,7 @@
         <v>60</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -4597,7 +4593,7 @@
         <v>59</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -4611,7 +4607,7 @@
         <v>61</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -4625,7 +4621,7 @@
         <v>62</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4656,7 +4652,7 @@
         <v>142</v>
       </c>
       <c r="G65" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -4673,7 +4669,7 @@
         <v>143</v>
       </c>
       <c r="G66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -4690,7 +4686,7 @@
         <v>155</v>
       </c>
       <c r="G67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -4704,10 +4700,10 @@
         <v>99</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>164</v>
+        <v>412</v>
       </c>
       <c r="G68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -4721,10 +4717,10 @@
         <v>100</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G69" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -4738,7 +4734,7 @@
         <v>101</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -4752,7 +4748,7 @@
         <v>102</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -4766,7 +4762,7 @@
         <v>64</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -4780,7 +4776,7 @@
         <v>105</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -4808,7 +4804,7 @@
         <v>66</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -4822,7 +4818,7 @@
         <v>68</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -4836,7 +4832,7 @@
         <v>74</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -4850,7 +4846,7 @@
         <v>67</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -4864,7 +4860,7 @@
         <v>70</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -4878,7 +4874,7 @@
         <v>73</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -4892,7 +4888,7 @@
         <v>108</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -4906,7 +4902,7 @@
         <v>76</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -4920,7 +4916,7 @@
         <v>63</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -4934,7 +4930,7 @@
         <v>69</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -4948,7 +4944,7 @@
         <v>72</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -4962,7 +4958,7 @@
         <v>107</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -4976,7 +4972,7 @@
         <v>71</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -4990,7 +4986,7 @@
         <v>75</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -5004,7 +5000,7 @@
         <v>78</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -5018,7 +5014,7 @@
         <v>80</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -5032,7 +5028,7 @@
         <v>77</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -5046,7 +5042,7 @@
         <v>79</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -5060,7 +5056,7 @@
         <v>82</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -5074,7 +5070,7 @@
         <v>81</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -5102,7 +5098,7 @@
         <v>83</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -5116,7 +5112,7 @@
         <v>84</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -5130,7 +5126,7 @@
         <v>85</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -5144,10 +5140,10 @@
         <v>104</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G99" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -5161,10 +5157,10 @@
         <v>103</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G100" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -5178,10 +5174,10 @@
         <v>106</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G101" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -5195,10 +5191,10 @@
         <v>109</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G102" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -5212,10 +5208,10 @@
         <v>110</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G103" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -5263,10 +5259,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" t="s">
         <v>208</v>
-      </c>
-      <c r="F2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5277,10 +5273,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F3" t="s">
         <v>253</v>
-      </c>
-      <c r="F3" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5291,10 +5287,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" t="s">
         <v>255</v>
-      </c>
-      <c r="F4" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5305,10 +5301,10 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F5" t="s">
         <v>210</v>
-      </c>
-      <c r="F5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5319,10 +5315,10 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" t="s">
         <v>212</v>
-      </c>
-      <c r="F6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5333,10 +5329,10 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -5347,10 +5343,10 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" t="s">
         <v>215</v>
-      </c>
-      <c r="F8" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -5361,10 +5357,10 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9" t="s">
         <v>217</v>
-      </c>
-      <c r="F9" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -5375,10 +5371,10 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" t="s">
         <v>219</v>
-      </c>
-      <c r="F10" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -5389,10 +5385,10 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
+        <v>220</v>
+      </c>
+      <c r="F11" t="s">
         <v>221</v>
-      </c>
-      <c r="F11" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -5403,10 +5399,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F12" t="s">
         <v>257</v>
-      </c>
-      <c r="F12" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5417,10 +5413,10 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
+        <v>258</v>
+      </c>
+      <c r="F13" t="s">
         <v>259</v>
-      </c>
-      <c r="F13" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -5431,10 +5427,10 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" t="s">
         <v>261</v>
-      </c>
-      <c r="F14" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -5445,10 +5441,10 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F15" t="s">
         <v>263</v>
-      </c>
-      <c r="F15" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -5459,10 +5455,10 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
+        <v>264</v>
+      </c>
+      <c r="F16" t="s">
         <v>265</v>
-      </c>
-      <c r="F16" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -5473,10 +5469,10 @@
         <v>15</v>
       </c>
       <c r="E17" t="s">
+        <v>266</v>
+      </c>
+      <c r="F17" t="s">
         <v>267</v>
-      </c>
-      <c r="F17" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -5487,10 +5483,10 @@
         <v>16</v>
       </c>
       <c r="E18" t="s">
+        <v>268</v>
+      </c>
+      <c r="F18" t="s">
         <v>269</v>
-      </c>
-      <c r="F18" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -5501,10 +5497,10 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
+        <v>270</v>
+      </c>
+      <c r="F19" t="s">
         <v>271</v>
-      </c>
-      <c r="F19" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -5515,10 +5511,10 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
+        <v>272</v>
+      </c>
+      <c r="F20" t="s">
         <v>273</v>
-      </c>
-      <c r="F20" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -5529,10 +5525,10 @@
         <v>19</v>
       </c>
       <c r="E21" t="s">
+        <v>274</v>
+      </c>
+      <c r="F21" t="s">
         <v>275</v>
-      </c>
-      <c r="F21" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -5543,10 +5539,10 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F22" t="s">
         <v>277</v>
-      </c>
-      <c r="F22" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -5557,10 +5553,10 @@
         <v>21</v>
       </c>
       <c r="E23" t="s">
+        <v>278</v>
+      </c>
+      <c r="F23" t="s">
         <v>279</v>
-      </c>
-      <c r="F23" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -5571,10 +5567,10 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
+        <v>280</v>
+      </c>
+      <c r="F24" t="s">
         <v>281</v>
-      </c>
-      <c r="F24" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -5585,10 +5581,10 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
+        <v>282</v>
+      </c>
+      <c r="F25" t="s">
         <v>283</v>
-      </c>
-      <c r="F25" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -5599,10 +5595,10 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
+        <v>284</v>
+      </c>
+      <c r="F26" t="s">
         <v>285</v>
-      </c>
-      <c r="F26" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -5613,10 +5609,10 @@
         <v>25</v>
       </c>
       <c r="E27" t="s">
+        <v>286</v>
+      </c>
+      <c r="F27" t="s">
         <v>287</v>
-      </c>
-      <c r="F27" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -5627,10 +5623,10 @@
         <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -5641,10 +5637,10 @@
         <v>27</v>
       </c>
       <c r="E29" t="s">
+        <v>289</v>
+      </c>
+      <c r="F29" t="s">
         <v>290</v>
-      </c>
-      <c r="F29" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -5655,10 +5651,10 @@
         <v>28</v>
       </c>
       <c r="E30" t="s">
+        <v>291</v>
+      </c>
+      <c r="F30" t="s">
         <v>292</v>
-      </c>
-      <c r="F30" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -5669,10 +5665,10 @@
         <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -5683,10 +5679,10 @@
         <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F32" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -5697,10 +5693,10 @@
         <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F33" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -5711,10 +5707,10 @@
         <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F34" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -5725,10 +5721,10 @@
         <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F35" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -5739,10 +5735,10 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
+        <v>293</v>
+      </c>
+      <c r="F36" t="s">
         <v>294</v>
-      </c>
-      <c r="F36" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -5753,10 +5749,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
+        <v>295</v>
+      </c>
+      <c r="F37" t="s">
         <v>296</v>
-      </c>
-      <c r="F37" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -5767,10 +5763,10 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" t="s">
         <v>223</v>
-      </c>
-      <c r="F38" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -5781,10 +5777,10 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
+        <v>224</v>
+      </c>
+      <c r="F39" t="s">
         <v>225</v>
-      </c>
-      <c r="F39" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -5795,10 +5791,10 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
+        <v>297</v>
+      </c>
+      <c r="F40" t="s">
         <v>298</v>
-      </c>
-      <c r="F40" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -5809,10 +5805,10 @@
         <v>5</v>
       </c>
       <c r="E41" t="s">
+        <v>226</v>
+      </c>
+      <c r="F41" t="s">
         <v>227</v>
-      </c>
-      <c r="F41" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -5823,10 +5819,10 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F42" t="s">
         <v>229</v>
-      </c>
-      <c r="F42" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -5837,10 +5833,10 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
+        <v>230</v>
+      </c>
+      <c r="F43" t="s">
         <v>231</v>
-      </c>
-      <c r="F43" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -5851,10 +5847,10 @@
         <v>8</v>
       </c>
       <c r="E44" t="s">
+        <v>232</v>
+      </c>
+      <c r="F44" t="s">
         <v>233</v>
-      </c>
-      <c r="F44" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -5865,10 +5861,10 @@
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F45" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -5879,10 +5875,10 @@
         <v>10</v>
       </c>
       <c r="E46" t="s">
+        <v>235</v>
+      </c>
+      <c r="F46" t="s">
         <v>236</v>
-      </c>
-      <c r="F46" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -5893,10 +5889,10 @@
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -5907,10 +5903,10 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
+        <v>300</v>
+      </c>
+      <c r="F48" t="s">
         <v>301</v>
-      </c>
-      <c r="F48" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -5921,10 +5917,10 @@
         <v>13</v>
       </c>
       <c r="E49" t="s">
+        <v>302</v>
+      </c>
+      <c r="F49" t="s">
         <v>303</v>
-      </c>
-      <c r="F49" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -5935,10 +5931,10 @@
         <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F50" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -5949,10 +5945,10 @@
         <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F51" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -5963,10 +5959,10 @@
         <v>16</v>
       </c>
       <c r="E52" t="s">
+        <v>305</v>
+      </c>
+      <c r="F52" t="s">
         <v>306</v>
-      </c>
-      <c r="F52" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -5977,10 +5973,10 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
+        <v>307</v>
+      </c>
+      <c r="F53" t="s">
         <v>308</v>
-      </c>
-      <c r="F53" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -5991,10 +5987,10 @@
         <v>18</v>
       </c>
       <c r="E54" t="s">
+        <v>309</v>
+      </c>
+      <c r="F54" t="s">
         <v>310</v>
-      </c>
-      <c r="F54" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -6005,10 +6001,10 @@
         <v>19</v>
       </c>
       <c r="E55" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F55" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -6019,10 +6015,10 @@
         <v>20</v>
       </c>
       <c r="E56" t="s">
+        <v>312</v>
+      </c>
+      <c r="F56" t="s">
         <v>313</v>
-      </c>
-      <c r="F56" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -6033,10 +6029,10 @@
         <v>21</v>
       </c>
       <c r="E57" t="s">
+        <v>314</v>
+      </c>
+      <c r="F57" t="s">
         <v>315</v>
-      </c>
-      <c r="F57" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -6047,10 +6043,10 @@
         <v>22</v>
       </c>
       <c r="E58" t="s">
+        <v>316</v>
+      </c>
+      <c r="F58" t="s">
         <v>317</v>
-      </c>
-      <c r="F58" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -6061,10 +6057,10 @@
         <v>23</v>
       </c>
       <c r="E59" t="s">
+        <v>318</v>
+      </c>
+      <c r="F59" t="s">
         <v>319</v>
-      </c>
-      <c r="F59" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -6075,10 +6071,10 @@
         <v>24</v>
       </c>
       <c r="E60" t="s">
+        <v>320</v>
+      </c>
+      <c r="F60" t="s">
         <v>321</v>
-      </c>
-      <c r="F60" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -6089,10 +6085,10 @@
         <v>25</v>
       </c>
       <c r="E61" t="s">
+        <v>322</v>
+      </c>
+      <c r="F61" t="s">
         <v>323</v>
-      </c>
-      <c r="F61" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -6103,10 +6099,10 @@
         <v>26</v>
       </c>
       <c r="E62" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F62" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -6117,10 +6113,10 @@
         <v>27</v>
       </c>
       <c r="E63" t="s">
+        <v>325</v>
+      </c>
+      <c r="F63" t="s">
         <v>326</v>
-      </c>
-      <c r="F63" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -6131,10 +6127,10 @@
         <v>28</v>
       </c>
       <c r="E64" t="s">
+        <v>327</v>
+      </c>
+      <c r="F64" t="s">
         <v>328</v>
-      </c>
-      <c r="F64" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -6145,10 +6141,10 @@
         <v>29</v>
       </c>
       <c r="E65" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F65" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -6159,10 +6155,10 @@
         <v>30</v>
       </c>
       <c r="E66" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F66" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -6173,10 +6169,10 @@
         <v>31</v>
       </c>
       <c r="E67" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F67" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -6187,10 +6183,10 @@
         <v>32</v>
       </c>
       <c r="E68" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F68" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -6201,10 +6197,10 @@
         <v>33</v>
       </c>
       <c r="E69" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F69" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -6215,10 +6211,10 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
+        <v>237</v>
+      </c>
+      <c r="F70" t="s">
         <v>238</v>
-      </c>
-      <c r="F70" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -6229,10 +6225,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
+        <v>329</v>
+      </c>
+      <c r="F71" t="s">
         <v>330</v>
-      </c>
-      <c r="F71" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -6243,10 +6239,10 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
+        <v>239</v>
+      </c>
+      <c r="F72" t="s">
         <v>240</v>
-      </c>
-      <c r="F72" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -6257,10 +6253,10 @@
         <v>3</v>
       </c>
       <c r="E73" t="s">
+        <v>241</v>
+      </c>
+      <c r="F73" t="s">
         <v>242</v>
-      </c>
-      <c r="F73" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -6271,10 +6267,10 @@
         <v>4</v>
       </c>
       <c r="E74" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F74" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -6285,10 +6281,10 @@
         <v>5</v>
       </c>
       <c r="E75" t="s">
+        <v>243</v>
+      </c>
+      <c r="F75" t="s">
         <v>244</v>
-      </c>
-      <c r="F75" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -6299,10 +6295,10 @@
         <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F76" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -6313,10 +6309,10 @@
         <v>7</v>
       </c>
       <c r="E77" t="s">
+        <v>332</v>
+      </c>
+      <c r="F77" t="s">
         <v>333</v>
-      </c>
-      <c r="F77" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -6327,10 +6323,10 @@
         <v>8</v>
       </c>
       <c r="E78" t="s">
+        <v>246</v>
+      </c>
+      <c r="F78" t="s">
         <v>247</v>
-      </c>
-      <c r="F78" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -6341,10 +6337,10 @@
         <v>9</v>
       </c>
       <c r="E79" t="s">
+        <v>248</v>
+      </c>
+      <c r="F79" t="s">
         <v>249</v>
-      </c>
-      <c r="F79" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -6355,10 +6351,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
+        <v>250</v>
+      </c>
+      <c r="F80" t="s">
         <v>251</v>
-      </c>
-      <c r="F80" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -6369,10 +6365,10 @@
         <v>11</v>
       </c>
       <c r="E81" t="s">
+        <v>334</v>
+      </c>
+      <c r="F81" t="s">
         <v>335</v>
-      </c>
-      <c r="F81" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -6383,10 +6379,10 @@
         <v>12</v>
       </c>
       <c r="E82" t="s">
+        <v>336</v>
+      </c>
+      <c r="F82" t="s">
         <v>337</v>
-      </c>
-      <c r="F82" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -6397,10 +6393,10 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
+        <v>338</v>
+      </c>
+      <c r="F83" t="s">
         <v>339</v>
-      </c>
-      <c r="F83" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -6411,10 +6407,10 @@
         <v>14</v>
       </c>
       <c r="E84" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F84" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -6425,10 +6421,10 @@
         <v>15</v>
       </c>
       <c r="E85" t="s">
+        <v>341</v>
+      </c>
+      <c r="F85" t="s">
         <v>342</v>
-      </c>
-      <c r="F85" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -6439,10 +6435,10 @@
         <v>16</v>
       </c>
       <c r="E86" t="s">
+        <v>343</v>
+      </c>
+      <c r="F86" t="s">
         <v>344</v>
-      </c>
-      <c r="F86" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -6453,10 +6449,10 @@
         <v>17</v>
       </c>
       <c r="E87" t="s">
+        <v>345</v>
+      </c>
+      <c r="F87" t="s">
         <v>346</v>
-      </c>
-      <c r="F87" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -6467,10 +6463,10 @@
         <v>18</v>
       </c>
       <c r="E88" t="s">
+        <v>347</v>
+      </c>
+      <c r="F88" t="s">
         <v>348</v>
-      </c>
-      <c r="F88" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -6481,10 +6477,10 @@
         <v>19</v>
       </c>
       <c r="E89" t="s">
+        <v>349</v>
+      </c>
+      <c r="F89" t="s">
         <v>350</v>
-      </c>
-      <c r="F89" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -6495,10 +6491,10 @@
         <v>20</v>
       </c>
       <c r="E90" t="s">
+        <v>351</v>
+      </c>
+      <c r="F90" t="s">
         <v>352</v>
-      </c>
-      <c r="F90" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -6509,10 +6505,10 @@
         <v>21</v>
       </c>
       <c r="E91" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F91" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -6523,10 +6519,10 @@
         <v>22</v>
       </c>
       <c r="E92" t="s">
+        <v>354</v>
+      </c>
+      <c r="F92" t="s">
         <v>355</v>
-      </c>
-      <c r="F92" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -6537,10 +6533,10 @@
         <v>23</v>
       </c>
       <c r="E93" t="s">
+        <v>356</v>
+      </c>
+      <c r="F93" t="s">
         <v>357</v>
-      </c>
-      <c r="F93" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -6551,10 +6547,10 @@
         <v>24</v>
       </c>
       <c r="E94" t="s">
+        <v>358</v>
+      </c>
+      <c r="F94" t="s">
         <v>359</v>
-      </c>
-      <c r="F94" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -6565,10 +6561,10 @@
         <v>25</v>
       </c>
       <c r="E95" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F95" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -6579,10 +6575,10 @@
         <v>26</v>
       </c>
       <c r="E96" t="s">
+        <v>361</v>
+      </c>
+      <c r="F96" t="s">
         <v>362</v>
-      </c>
-      <c r="F96" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -6593,10 +6589,10 @@
         <v>27</v>
       </c>
       <c r="E97" t="s">
+        <v>363</v>
+      </c>
+      <c r="F97" t="s">
         <v>364</v>
-      </c>
-      <c r="F97" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -6607,10 +6603,10 @@
         <v>28</v>
       </c>
       <c r="E98" t="s">
+        <v>365</v>
+      </c>
+      <c r="F98" t="s">
         <v>366</v>
-      </c>
-      <c r="F98" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -6621,10 +6617,10 @@
         <v>29</v>
       </c>
       <c r="E99" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F99" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -6635,10 +6631,10 @@
         <v>30</v>
       </c>
       <c r="E100" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F100" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -6649,10 +6645,10 @@
         <v>31</v>
       </c>
       <c r="E101" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F101" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -6663,10 +6659,10 @@
         <v>32</v>
       </c>
       <c r="E102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F102" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -6677,10 +6673,10 @@
         <v>33</v>
       </c>
       <c r="E103" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F103" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: cs, pl i18n complete (#9)
</commit_message>
<xml_diff>
--- a/tools/data-processing/data.xlsx
+++ b/tools/data-processing/data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\might-and-magic\arcomage-hd\tools\data-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA902BF-CFBD-497A-BB97-3BFFBD629D38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7051CA-1ADB-4BC9-8033-1D7AC1F5EC88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="4" r:id="rId1"/>
     <sheet name="cards.en" sheetId="2" r:id="rId2"/>
     <sheet name="cards.zh-Hans" sheetId="3" r:id="rId3"/>
+    <sheet name="cards.pl" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="614">
   <si>
     <t>Type</t>
   </si>
@@ -1266,6 +1267,609 @@
   </si>
   <si>
     <t>If Tower &gt; enemy wall, 8 damage to enemy tower. Else 8 damage</t>
+  </si>
+  <si>
+    <t>Deficyt Kamieni</t>
+  </si>
+  <si>
+    <t>Wszyscy gracze tracą 8 kamieni</t>
+  </si>
+  <si>
+    <t>Szczęśliwy Traf</t>
+  </si>
+  <si>
+    <t>+2 kamienie. +2 klejnoty. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Przyjazny Teren</t>
+  </si>
+  <si>
+    <t>+1 Mur. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Górnicy</t>
+  </si>
+  <si>
+    <t>+1 Warsztat</t>
+  </si>
+  <si>
+    <t>Wielki Ładunek</t>
+  </si>
+  <si>
+    <t>Jeżeli Warsztat &lt; Warsztat przeciwnika, to Warsztat +2, inaczej Warsztat +1</t>
+  </si>
+  <si>
+    <t>Krasnoludzcy Górnicy</t>
+  </si>
+  <si>
+    <t>+4 Mur. +1 Warsztat</t>
+  </si>
+  <si>
+    <t>Praca po Godzinach</t>
+  </si>
+  <si>
+    <t>+5 Mur. tracisz 6 klejnotów</t>
+  </si>
+  <si>
+    <t>Kopiowanie Planów</t>
+  </si>
+  <si>
+    <t>Jeżeli Warsztat &lt; Warsztat przeciwnika, to Warsztat = Warsztat przeciwnika</t>
+  </si>
+  <si>
+    <t>Podstawowy Mur</t>
+  </si>
+  <si>
+    <t>+3 Mur</t>
+  </si>
+  <si>
+    <t>Mocny Mur</t>
+  </si>
+  <si>
+    <t>+4 Mur</t>
+  </si>
+  <si>
+    <t>Wzmocniony Mur</t>
+  </si>
+  <si>
+    <t>+8 Mur</t>
+  </si>
+  <si>
+    <t>Kopalnia Rozbiórkowa</t>
+  </si>
+  <si>
+    <t>-1 Warsztat. +10 Mur. +5 klejnotów</t>
+  </si>
+  <si>
+    <t>Nowe Narzędzia</t>
+  </si>
+  <si>
+    <t>+2 Warsztat</t>
+  </si>
+  <si>
+    <t>Runięcie</t>
+  </si>
+  <si>
+    <t>-1 Warsztat przeciwnika</t>
+  </si>
+  <si>
+    <t>Duży Mur</t>
+  </si>
+  <si>
+    <t>+6 Mur</t>
+  </si>
+  <si>
+    <t>Trzęsienie Ziemi</t>
+  </si>
+  <si>
+    <t>-1 Warsztat dla wszystkich graczy</t>
+  </si>
+  <si>
+    <t>Tajemniczy Pokój</t>
+  </si>
+  <si>
+    <t>+1 Magia. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Wstrząsy</t>
+  </si>
+  <si>
+    <t>-5 Mury wszystkich graczy. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Fundamenty</t>
+  </si>
+  <si>
+    <t>Jeżeli Wysokość twojego Muru = 0, to Mur +6, inaczej Mur +3</t>
+  </si>
+  <si>
+    <t>Innowacje</t>
+  </si>
+  <si>
+    <t>+1 Warsztaty wszystkich graczy. +4 klejnoty</t>
+  </si>
+  <si>
+    <t>Brama</t>
+  </si>
+  <si>
+    <t>+5 Mur. +1 Lochy</t>
+  </si>
+  <si>
+    <t>Kryształowe Skały</t>
+  </si>
+  <si>
+    <t>+7 Mur. +7 klejnotów</t>
+  </si>
+  <si>
+    <t>Dźwięcząca Ruda</t>
+  </si>
+  <si>
+    <t>+6 Mur. +3 Wieża</t>
+  </si>
+  <si>
+    <t>Wielki Mur</t>
+  </si>
+  <si>
+    <t>+12 Mur</t>
+  </si>
+  <si>
+    <t>Dokładne Projekty</t>
+  </si>
+  <si>
+    <t>+8 Mur. +5 Wieża</t>
+  </si>
+  <si>
+    <t>Wspaniały Mur</t>
+  </si>
+  <si>
+    <t>+15 Mur</t>
+  </si>
+  <si>
+    <t>Wyrzutnia Kamieni</t>
+  </si>
+  <si>
+    <t>+6 Mur. 10 obrażeń wrogowi</t>
+  </si>
+  <si>
+    <t>Serce Smoka</t>
+  </si>
+  <si>
+    <t>+20 Mur. +8 Wieża</t>
+  </si>
+  <si>
+    <t>Przymusowa Praca</t>
+  </si>
+  <si>
+    <t>+9 Mur. -5 bestii</t>
+  </si>
+  <si>
+    <t>Kamienny Ogród</t>
+  </si>
+  <si>
+    <t>+1 Mur. +1 Wieża. +2 bestie</t>
+  </si>
+  <si>
+    <t>Fala Powodziowa</t>
+  </si>
+  <si>
+    <t>Gracz(e) z najniższym murem otrzymują -1 Lochy i 2 obrażeń wieży</t>
+  </si>
+  <si>
+    <t>Koszary</t>
+  </si>
+  <si>
+    <t>+6 bestii. +6 Mur. Jeżeli Lochy &lt; Lochy przeciwnika, to Lochy +1</t>
+  </si>
+  <si>
+    <t>Fortyfikacje</t>
+  </si>
+  <si>
+    <t>+7 Mur. 6 obrażeń wrogowi</t>
+  </si>
+  <si>
+    <t>Zamiana</t>
+  </si>
+  <si>
+    <t>Zamień miejscami twój mur z murem przeciwnika</t>
+  </si>
+  <si>
+    <t>Kwarc</t>
+  </si>
+  <si>
+    <t>+1 Wieża. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Kwarc Dymny</t>
+  </si>
+  <si>
+    <t>1 obrażenie Wieży przeciwnika. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Amestyt</t>
+  </si>
+  <si>
+    <t>+3 Wieża</t>
+  </si>
+  <si>
+    <t>Tkacze Zaklęć</t>
+  </si>
+  <si>
+    <t>+1 Magia</t>
+  </si>
+  <si>
+    <t>Pryzmat</t>
+  </si>
+  <si>
+    <t>Niebezpieczny Kamień</t>
+  </si>
+  <si>
+    <t>+3 Wieża. tej karty nie można odłożyć bez zagrania nią</t>
+  </si>
+  <si>
+    <t>Słoneczny Błysk</t>
+  </si>
+  <si>
+    <t>+2 Wieża. 2 obrażenia Wieży wroga</t>
+  </si>
+  <si>
+    <t>Kryształowa Matryca</t>
+  </si>
+  <si>
+    <t>+1 Magia. +3 Wieża. +1 Wieża przeciwnika</t>
+  </si>
+  <si>
+    <t>Skaza Kamieni Szlachetnych</t>
+  </si>
+  <si>
+    <t>3 obrażenia Wieży przeciwnika</t>
+  </si>
+  <si>
+    <t>Rubin</t>
+  </si>
+  <si>
+    <t>+5 Wieża</t>
+  </si>
+  <si>
+    <t>Szmaragdowa Włócznia</t>
+  </si>
+  <si>
+    <t>5 obrażeń Wieży przeciwnika</t>
+  </si>
+  <si>
+    <t>Energetyczne Spalenie</t>
+  </si>
+  <si>
+    <t>5 obrażeń twojej Wieży. +2 Magia</t>
+  </si>
+  <si>
+    <t>Harmoniczne Wibracje</t>
+  </si>
+  <si>
+    <t>+1 Magia. +3 Wieża. +3 Mur</t>
+  </si>
+  <si>
+    <t>Równowaga</t>
+  </si>
+  <si>
+    <t>Magia wszystkich graczy staje się równa Magii temu, który ma jej najwięcej</t>
+  </si>
+  <si>
+    <t>Szmaragd</t>
+  </si>
+  <si>
+    <t>+8 Wieża</t>
+  </si>
+  <si>
+    <t>Perła Mąrdości</t>
+  </si>
+  <si>
+    <t>+5 Wieża. +1 Magia</t>
+  </si>
+  <si>
+    <t>Niszczyciel</t>
+  </si>
+  <si>
+    <t>-1 Magia. 9 obrażeń Wieży przeciwnika</t>
+  </si>
+  <si>
+    <t>Kruchy Kamień</t>
+  </si>
+  <si>
+    <t>+5 Wieża. przeciwnik traci 6 kamieni</t>
+  </si>
+  <si>
+    <t>Szafir</t>
+  </si>
+  <si>
+    <t>+11 Wieża</t>
+  </si>
+  <si>
+    <t>Niezgoda</t>
+  </si>
+  <si>
+    <t>7 obrażeń wszystkim Wieżom. -1 Magia wszystkich graczy</t>
+  </si>
+  <si>
+    <t>Ognisty Rubin</t>
+  </si>
+  <si>
+    <t>Pomocnik Warsztatu</t>
+  </si>
+  <si>
+    <t>+7 Wieża. -10 kamieni</t>
+  </si>
+  <si>
+    <t>Kryształowa Tarcza</t>
+  </si>
+  <si>
+    <t>+8 Wieża. +3 Mur</t>
+  </si>
+  <si>
+    <t>Klejnot Empatii</t>
+  </si>
+  <si>
+    <t>+8 Wieża. +1 Lochy</t>
+  </si>
+  <si>
+    <t>Diament</t>
+  </si>
+  <si>
+    <t>+15 Wieża</t>
+  </si>
+  <si>
+    <t>Sanktuarium</t>
+  </si>
+  <si>
+    <t>+10 Wieża. +5 Mur. +5 bestii</t>
+  </si>
+  <si>
+    <t>Magmowy Klejnot</t>
+  </si>
+  <si>
+    <t>+12 Wieża. 6 obrażeń wszystkim wrogom</t>
+  </si>
+  <si>
+    <t>Oko Smoka</t>
+  </si>
+  <si>
+    <t>+20 Wieża</t>
+  </si>
+  <si>
+    <t>Krystalizacja</t>
+  </si>
+  <si>
+    <t>+11 Wieża. -6 Mur</t>
+  </si>
+  <si>
+    <t>Trzos Świecidełek</t>
+  </si>
+  <si>
+    <t>Jeżeli Wieża &lt; Wieża przeciwnika, to +2 Wieża, inaczej +1 Wieża</t>
+  </si>
+  <si>
+    <t>Tęcza</t>
+  </si>
+  <si>
+    <t>+1 Wieże wszystkich graczy. +3 klejnoty</t>
+  </si>
+  <si>
+    <t>Uczennica</t>
+  </si>
+  <si>
+    <t>+4 Wieża. -3 bestie. 2 obrażenia Wieży przeciwnika</t>
+  </si>
+  <si>
+    <t>Błyskawica</t>
+  </si>
+  <si>
+    <t>Fazowy Klejnot</t>
+  </si>
+  <si>
+    <t>+13 Wieża. +6 bestii. +6 kamieni</t>
+  </si>
+  <si>
+    <t>Choroba Wściekłych Krów</t>
+  </si>
+  <si>
+    <t>-6 bestii dla wszystkich graczy</t>
+  </si>
+  <si>
+    <t>Driada</t>
+  </si>
+  <si>
+    <t>2 obrażenia. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Humorzaste Gobliny</t>
+  </si>
+  <si>
+    <t>4 obrażenia. -3 klejnoty</t>
+  </si>
+  <si>
+    <t>+1 Lochy</t>
+  </si>
+  <si>
+    <t>Elficki Zwiadowca</t>
+  </si>
+  <si>
+    <t>Banda Goblinów</t>
+  </si>
+  <si>
+    <t>6 obrażeń. otrzymujesz 3 obrażenia</t>
+  </si>
+  <si>
+    <t>Goblińscy Łucznicy</t>
+  </si>
+  <si>
+    <t>3 obrażenia Wieży wroga. otrzymujesz 1 obrażenie</t>
+  </si>
+  <si>
+    <t>Driada Cienia</t>
+  </si>
+  <si>
+    <t>2 obrażenia Wieży przeciwnika. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Ork</t>
+  </si>
+  <si>
+    <t>5 obrażeń</t>
+  </si>
+  <si>
+    <t>Krasnoludy</t>
+  </si>
+  <si>
+    <t>4 obrażenia. +3 Mur</t>
+  </si>
+  <si>
+    <t>Małe Węże</t>
+  </si>
+  <si>
+    <t>4 obrażenia Wieży przeciwnika</t>
+  </si>
+  <si>
+    <t>Trener Troli</t>
+  </si>
+  <si>
+    <t>+2 Lochy</t>
+  </si>
+  <si>
+    <t>Gremlin z Wieży</t>
+  </si>
+  <si>
+    <t>2 obrażenia. +4 Mur. +2 Wieża</t>
+  </si>
+  <si>
+    <t>Pełnia Księżyca</t>
+  </si>
+  <si>
+    <t>+1 Lochy wszystkich graczy. +3 bestie</t>
+  </si>
+  <si>
+    <t>Miecznik</t>
+  </si>
+  <si>
+    <t>6 obrażeń</t>
+  </si>
+  <si>
+    <t>Ogr</t>
+  </si>
+  <si>
+    <t>7 obrażeń</t>
+  </si>
+  <si>
+    <t>Szalone Owce</t>
+  </si>
+  <si>
+    <t>6 obrażeń. wróg traci 3 bestie</t>
+  </si>
+  <si>
+    <t>Diablik</t>
+  </si>
+  <si>
+    <t>6 obrażeń. -5 bestii, kamieni i klejnotów dla wszystkich graczy</t>
+  </si>
+  <si>
+    <t>Trutnie</t>
+  </si>
+  <si>
+    <t>Jeżeli Mur przeciwnika = 0 to 10 obrażeń, inaczej 6 obrażeń</t>
+  </si>
+  <si>
+    <t>Wilkołak</t>
+  </si>
+  <si>
+    <t>9 obrażeń</t>
+  </si>
+  <si>
+    <t>Chmura Korozji</t>
+  </si>
+  <si>
+    <t>Jeżeli Mur przeciwnika &gt; 0 to 10 obrażeń, inaczej 7 obrażeń</t>
+  </si>
+  <si>
+    <t>Jednorożec</t>
+  </si>
+  <si>
+    <t>Jeżeli Magia &gt; Magia przeciwnika to 12 obrażeń, inaczej 8 obrażeń</t>
+  </si>
+  <si>
+    <t>Elficcy Łucznicy</t>
+  </si>
+  <si>
+    <t>Jeżeli Mur &gt; Mur przeciwnika to 6 obrażeń Wieży przeciwnika, inaczej 6 obrażeń</t>
+  </si>
+  <si>
+    <t>Sukub</t>
+  </si>
+  <si>
+    <t>5 obrażeń Wieży przeciwnika,. wróg traci 8 bestii</t>
+  </si>
+  <si>
+    <t>Niszczyciele Skał</t>
+  </si>
+  <si>
+    <t>8 obrażeń. -1 Warsztat przeciwnika</t>
+  </si>
+  <si>
+    <t>Złodziej</t>
+  </si>
+  <si>
+    <t>Skalny Kolos</t>
+  </si>
+  <si>
+    <t>10 obrażeń. +4 Mur</t>
+  </si>
+  <si>
+    <t>Wampir</t>
+  </si>
+  <si>
+    <t>10 obrażeń. wróg traci 5 bestii. -1 Lochy przeciwnika</t>
+  </si>
+  <si>
+    <t>Smok</t>
+  </si>
+  <si>
+    <t>20 obrażeń. przeciwnik traci 10 klejnotów. -1 Lochy przeciwnika</t>
+  </si>
+  <si>
+    <t>Włócznik</t>
+  </si>
+  <si>
+    <t>Jeżeli Mur &gt; Mur przeciwnika to 3 obrażenia, inaczej 2 obrażenia</t>
+  </si>
+  <si>
+    <t>Gnom</t>
+  </si>
+  <si>
+    <t>3 obrażenia. +1 klejnot</t>
+  </si>
+  <si>
+    <t>8 obrażeń. 3 obrażenia twojej Wieży</t>
+  </si>
+  <si>
+    <t>Watażka</t>
+  </si>
+  <si>
+    <t>13 obrażeń. -3 klejnoty</t>
+  </si>
+  <si>
+    <t>Jeździec Pegaza</t>
+  </si>
+  <si>
+    <t>12 obrażeń Wieży przeciwnika</t>
+  </si>
+  <si>
+    <t>Odłóż jedną kartę. dobierz jedną kartę. dodatkowy ruch</t>
+  </si>
+  <si>
+    <t>Jeżeli Wieża &gt; Wieża przeciwnika to 8 obrażeń Wieży przeciwnika, inaczej 8 obrażeń przeciwnikowi</t>
+  </si>
+  <si>
+    <t>Wróg traci 10 klejnotów i 5 kamieni. ty zyskujesz połowę z tego (liczby zaokrąglone w górę)</t>
+  </si>
+  <si>
+    <t>+6 Wieża. 4 obrażenia wszystkim wrogim Wieżom</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +2190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399247F-B0D6-4509-8DB3-900582E8810F}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3714,7 +4318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C56CEB-8692-4AC2-8CE6-B1BDDA007E98}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6682,4 +7288,1470 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC409FE-2D06-4F59-A0F8-08433C7430B4}">
+  <dimension ref="A1:F103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.88671875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>417</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>419</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>421</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>423</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>425</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>427</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>429</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>431</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>451</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>449</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>447</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>445</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>443</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>441</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>439</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>437</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>435</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>433</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>453</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>455</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>457</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>459</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>461</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>463</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>465</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>467</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>469</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>471</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>473</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="E33" t="s">
+        <v>475</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>477</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>479</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>481</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>483</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>485</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>487</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>489</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>490</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>492</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>494</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>496</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>498</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
+        <v>500</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>502</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s">
+        <v>504</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s">
+        <v>506</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s">
+        <v>508</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>15</v>
+      </c>
+      <c r="E51" t="s">
+        <v>510</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>512</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>514</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>516</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>19</v>
+      </c>
+      <c r="E55" t="s">
+        <v>518</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>20</v>
+      </c>
+      <c r="E56" t="s">
+        <v>520</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>21</v>
+      </c>
+      <c r="E57" t="s">
+        <v>521</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>22</v>
+      </c>
+      <c r="E58" t="s">
+        <v>523</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>23</v>
+      </c>
+      <c r="E59" t="s">
+        <v>525</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>24</v>
+      </c>
+      <c r="E60" t="s">
+        <v>527</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>25</v>
+      </c>
+      <c r="E61" t="s">
+        <v>529</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>26</v>
+      </c>
+      <c r="E62" t="s">
+        <v>531</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>27</v>
+      </c>
+      <c r="E63" t="s">
+        <v>533</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>28</v>
+      </c>
+      <c r="E64" t="s">
+        <v>535</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>29</v>
+      </c>
+      <c r="E65" t="s">
+        <v>537</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>30</v>
+      </c>
+      <c r="E66" t="s">
+        <v>539</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>31</v>
+      </c>
+      <c r="E67" t="s">
+        <v>541</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>32</v>
+      </c>
+      <c r="E68" t="s">
+        <v>543</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>33</v>
+      </c>
+      <c r="E69" t="s">
+        <v>544</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>546</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>548</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
+        <v>550</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>105</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="E74" t="s">
+        <v>553</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>554</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>2</v>
+      </c>
+      <c r="B76">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
+        <v>556</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+      <c r="E77" t="s">
+        <v>558</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78">
+        <v>8</v>
+      </c>
+      <c r="E78" t="s">
+        <v>560</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>562</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>2</v>
+      </c>
+      <c r="B80">
+        <v>10</v>
+      </c>
+      <c r="E80" t="s">
+        <v>564</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81">
+        <v>11</v>
+      </c>
+      <c r="E81" t="s">
+        <v>566</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>2</v>
+      </c>
+      <c r="B82">
+        <v>12</v>
+      </c>
+      <c r="E82" t="s">
+        <v>568</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="B83">
+        <v>13</v>
+      </c>
+      <c r="E83" t="s">
+        <v>570</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="B84">
+        <v>14</v>
+      </c>
+      <c r="E84" t="s">
+        <v>572</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>2</v>
+      </c>
+      <c r="B85">
+        <v>15</v>
+      </c>
+      <c r="E85" t="s">
+        <v>574</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2</v>
+      </c>
+      <c r="B86">
+        <v>16</v>
+      </c>
+      <c r="E86" t="s">
+        <v>576</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>2</v>
+      </c>
+      <c r="B87">
+        <v>17</v>
+      </c>
+      <c r="E87" t="s">
+        <v>578</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88">
+        <v>18</v>
+      </c>
+      <c r="E88" t="s">
+        <v>580</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>2</v>
+      </c>
+      <c r="B89">
+        <v>19</v>
+      </c>
+      <c r="E89" t="s">
+        <v>582</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <v>20</v>
+      </c>
+      <c r="E90" t="s">
+        <v>584</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>2</v>
+      </c>
+      <c r="B91">
+        <v>21</v>
+      </c>
+      <c r="E91" t="s">
+        <v>586</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2</v>
+      </c>
+      <c r="B92">
+        <v>22</v>
+      </c>
+      <c r="E92" t="s">
+        <v>588</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="B93">
+        <v>23</v>
+      </c>
+      <c r="E93" t="s">
+        <v>590</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <v>24</v>
+      </c>
+      <c r="E94" t="s">
+        <v>592</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>2</v>
+      </c>
+      <c r="B95">
+        <v>25</v>
+      </c>
+      <c r="E95" t="s">
+        <v>594</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96">
+        <v>26</v>
+      </c>
+      <c r="E96" t="s">
+        <v>595</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>2</v>
+      </c>
+      <c r="B97">
+        <v>27</v>
+      </c>
+      <c r="E97" t="s">
+        <v>597</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>28</v>
+      </c>
+      <c r="E98" t="s">
+        <v>599</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99">
+        <v>29</v>
+      </c>
+      <c r="E99" t="s">
+        <v>601</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100">
+        <v>30</v>
+      </c>
+      <c r="E100" t="s">
+        <v>603</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="B101">
+        <v>31</v>
+      </c>
+      <c r="E101" t="s">
+        <v>106</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>32</v>
+      </c>
+      <c r="E102" t="s">
+        <v>606</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>2</v>
+      </c>
+      <c r="B103">
+        <v>33</v>
+      </c>
+      <c r="E103" t="s">
+        <v>608</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>